<commit_message>
LastEdit Index DataBase | 31-12-2023
</commit_message>
<xml_diff>
--- a/public/assets/files/ImportExcel.xlsx
+++ b/public/assets/files/ImportExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\prisoners_project\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE90C164-0B64-4CD2-B450-ED9F89EAF30E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76362C11-1240-428D-993B-A162581E7675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -323,7 +323,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="16"/>
       <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -354,7 +354,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,7 +638,7 @@
   <dimension ref="A1:AM3"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,7 +802,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:39" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -921,101 +921,101 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>234234234</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="3" spans="1:39" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="B3" s="1">
+        <v>99999999999</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>46</v>
       </c>
       <c r="H3" s="3">
         <v>36412</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="1" t="s">
         <v>48</v>
       </c>
       <c r="K3" s="3">
         <v>40461</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="1">
         <v>1</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="1">
         <v>2</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="1">
         <v>5</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="X3">
+      <c r="X3" s="1">
         <v>3</v>
       </c>
-      <c r="Y3">
+      <c r="Y3" s="1">
         <v>1</v>
       </c>
-      <c r="Z3">
+      <c r="Z3" s="1">
         <v>0</v>
       </c>
-      <c r="AA3">
+      <c r="AA3" s="1">
         <v>1</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AB3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AC3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AD3">
+      <c r="AD3" s="1">
         <v>2</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AE3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AF3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AG3" s="1" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
GoogleForm & ReviewData | 01-01-2024
</commit_message>
<xml_diff>
--- a/public/assets/files/ImportExcel.xlsx
+++ b/public/assets/files/ImportExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\prisoners_project\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76362C11-1240-428D-993B-A162581E7675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F58E0FE-970A-4C12-8FC6-3EE06AC4A260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="89">
   <si>
     <t>id</t>
   </si>
@@ -132,9 +132,6 @@
     <t>الانتماء</t>
   </si>
   <si>
-    <t>الحالة الصحية</t>
-  </si>
-  <si>
     <t>الحالة الاجتماعية</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
     <t>وحيد والديه,أمراض مزمنه,أقارب معتقلين</t>
   </si>
   <si>
-    <t>سرطان,بتر أعضاء,سكري</t>
-  </si>
-  <si>
     <t>father_arrested</t>
   </si>
   <si>
@@ -261,21 +255,6 @@
     <t>دبلوم</t>
   </si>
   <si>
-    <t>التخصص</t>
-  </si>
-  <si>
-    <t>specialization_name</t>
-  </si>
-  <si>
-    <t>برمجة ويب</t>
-  </si>
-  <si>
-    <t>university_name</t>
-  </si>
-  <si>
-    <t>اسم الجامعة</t>
-  </si>
-  <si>
     <t>first_phone_owner</t>
   </si>
   <si>
@@ -297,10 +276,22 @@
     <t>prisoner_type</t>
   </si>
   <si>
-    <t>health</t>
-  </si>
-  <si>
     <t>أسرى قدامى,أسرى مرضى</t>
+  </si>
+  <si>
+    <t>البلدة</t>
+  </si>
+  <si>
+    <t>town_id</t>
+  </si>
+  <si>
+    <t>health_note</t>
+  </si>
+  <si>
+    <t>وصف المرض</t>
+  </si>
+  <si>
+    <t>لا يوجد</t>
   </si>
 </sst>
 </file>
@@ -316,14 +307,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
+      <b/>
+      <sz val="18"/>
       <color theme="5" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -635,55 +628,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AM3"/>
+  <dimension ref="A1:AL3"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="28" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="26.5703125" customWidth="1"/>
-    <col min="33" max="33" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="50.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:38" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -703,7 +694,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -715,94 +706,91 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="Z1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="AF1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AG1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="AK1" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AM1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:39" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:38" s="2" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -813,7 +801,7 @@
         <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>24</v>
@@ -822,7 +810,7 @@
         <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>26</v>
@@ -834,192 +822,187 @@
         <v>28</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AG2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AI2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>40</v>
-      </c>
     </row>
-    <row r="3" spans="1:39" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:38" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>99999999999</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H3" s="3">
         <v>36412</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="3">
+        <v>40461</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K3" s="3">
-        <v>40461</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <v>2</v>
+      </c>
+      <c r="P3" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M3" s="1">
+      <c r="R3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z3" s="1">
         <v>1</v>
       </c>
-      <c r="N3" s="1">
+      <c r="AA3" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE3" s="1">
         <v>2</v>
       </c>
-      <c r="O3" s="1">
-        <v>5</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="X3" s="1">
-        <v>3</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB3" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC3" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD3" s="1">
-        <v>2</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="AF3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AG3" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
last updates before firing the website | 30-01-2024
</commit_message>
<xml_diff>
--- a/public/assets/files/ImportExcel.xlsx
+++ b/public/assets/files/ImportExcel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\prisoners_project\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F58E0FE-970A-4C12-8FC6-3EE06AC4A260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB77DDC-82B6-4BAC-AEEB-B42D31B906EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="93">
   <si>
     <t>id</t>
   </si>
@@ -292,6 +292,18 @@
   </si>
   <si>
     <t>لا يوجد</t>
+  </si>
+  <si>
+    <t>nick_name</t>
+  </si>
+  <si>
+    <t>الكنية</t>
+  </si>
+  <si>
+    <t>IsReleased</t>
+  </si>
+  <si>
+    <t>مفرج عنه؟</t>
   </si>
 </sst>
 </file>
@@ -628,9 +640,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL3"/>
+  <dimension ref="A1:AN3"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AL3" sqref="AL3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -640,41 +654,41 @@
     <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="33" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="50.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -697,100 +711,106 @@
         <v>42</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:38" s="2" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" s="2" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -813,100 +833,106 @@
         <v>43</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AK2" s="2" t="s">
+      <c r="AL2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="AL2" s="2" t="s">
+      <c r="AM2" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN2" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:38" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>99999999999</v>
       </c>
@@ -925,79 +951,82 @@
       <c r="G3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="3">
         <v>36412</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="3">
         <v>40461</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>1</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="1">
         <v>2</v>
       </c>
-      <c r="P3" s="1">
+      <c r="Q3" s="1">
         <v>5</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="V3" s="1" t="s">
         <v>55</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="Y3" s="1">
+      <c r="Y3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z3" s="1">
         <v>3</v>
       </c>
-      <c r="Z3" s="1">
+      <c r="AA3" s="1">
         <v>1</v>
       </c>
-      <c r="AA3" s="1">
+      <c r="AB3" s="1">
         <v>0</v>
       </c>
-      <c r="AB3" s="1">
+      <c r="AC3" s="1">
         <v>1</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AD3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AE3" s="1">
+      <c r="AF3" s="1">
         <v>2</v>
       </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AG3" s="1" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Firing the website | 01-02-2024
</commit_message>
<xml_diff>
--- a/public/assets/files/ImportExcel.xlsx
+++ b/public/assets/files/ImportExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\prisoners_project\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB77DDC-82B6-4BAC-AEEB-B42D31B906EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2714A6-14B5-445E-BE2D-5DEF5D3E8BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>id</t>
   </si>
@@ -162,39 +162,18 @@
     <t>اسم الأب</t>
   </si>
   <si>
-    <t>مثال</t>
-  </si>
-  <si>
-    <t>ذكر</t>
-  </si>
-  <si>
-    <t>نابلس</t>
-  </si>
-  <si>
-    <t>محكوم</t>
-  </si>
-  <si>
-    <t>حماس</t>
-  </si>
-  <si>
     <t>special_case</t>
   </si>
   <si>
     <t>حالة خاصة</t>
   </si>
   <si>
-    <t>وحيد والديه,أمراض مزمنه,أقارب معتقلين</t>
-  </si>
-  <si>
     <t>father_arrested</t>
   </si>
   <si>
     <t>الأب معتقل</t>
   </si>
   <si>
-    <t>نعم</t>
-  </si>
-  <si>
     <t>mother_arrested</t>
   </si>
   <si>
@@ -207,9 +186,6 @@
     <t>الزوجة معتقله</t>
   </si>
   <si>
-    <t>لا</t>
-  </si>
-  <si>
     <t>wife_arrested</t>
   </si>
   <si>
@@ -240,21 +216,12 @@
     <t>بنات معتقلين</t>
   </si>
   <si>
-    <t>متزوج</t>
-  </si>
-  <si>
-    <t>زوجة واحدة</t>
-  </si>
-  <si>
     <t>education_level</t>
   </si>
   <si>
     <t>المستوى التعليمي</t>
   </si>
   <si>
-    <t>دبلوم</t>
-  </si>
-  <si>
     <t>first_phone_owner</t>
   </si>
   <si>
@@ -276,9 +243,6 @@
     <t>prisoner_type</t>
   </si>
   <si>
-    <t>أسرى قدامى,أسرى مرضى</t>
-  </si>
-  <si>
     <t>البلدة</t>
   </si>
   <si>
@@ -291,9 +255,6 @@
     <t>وصف المرض</t>
   </si>
   <si>
-    <t>لا يوجد</t>
-  </si>
-  <si>
     <t>nick_name</t>
   </si>
   <si>
@@ -304,6 +265,12 @@
   </si>
   <si>
     <t>مفرج عنه؟</t>
+  </si>
+  <si>
+    <t>تاريخ الإفراج</t>
+  </si>
+  <si>
+    <t>arrest_end_date</t>
   </si>
 </sst>
 </file>
@@ -355,11 +322,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN3"/>
+  <dimension ref="A1:AO2"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AL3" sqref="AL3"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,35 +626,36 @@
     <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="27" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="39" max="40" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27" customWidth="1"/>
+    <col min="15" max="15" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="33" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="50.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -711,7 +678,7 @@
         <v>42</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -723,94 +690,97 @@
         <v>8</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="T1" s="1" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="AN1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:40" s="2" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:41" s="2" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -833,7 +803,7 @@
         <v>43</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>26</v>
@@ -845,189 +815,94 @@
         <v>28</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>40</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="U2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="W2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="X2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AM2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AD2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AE2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AL2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AM2" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="AN2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AO2" s="2" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:40" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B3" s="1">
-        <v>99999999999</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="3">
-        <v>36412</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M3" s="3">
-        <v>40461</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" s="1">
-        <v>1</v>
-      </c>
-      <c r="P3" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>5</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z3" s="1">
-        <v>3</v>
-      </c>
-      <c r="AA3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF3" s="1">
-        <v>2</v>
-      </c>
-      <c r="AG3" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
index is ready | 02-02-2024
</commit_message>
<xml_diff>
--- a/public/assets/files/ImportExcel.xlsx
+++ b/public/assets/files/ImportExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\prisoners_project\public\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2714A6-14B5-445E-BE2D-5DEF5D3E8BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD4E202-3324-44D7-AE53-D12BC7D5479D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -261,16 +261,16 @@
     <t>الكنية</t>
   </si>
   <si>
-    <t>IsReleased</t>
-  </si>
-  <si>
-    <t>مفرج عنه؟</t>
-  </si>
-  <si>
     <t>تاريخ الإفراج</t>
   </si>
   <si>
     <t>arrest_end_date</t>
+  </si>
+  <si>
+    <t>is_released</t>
+  </si>
+  <si>
+    <t>مفرج عنه</t>
   </si>
 </sst>
 </file>
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO2"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,7 +696,7 @@
         <v>9</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>10</v>
@@ -774,7 +774,7 @@
         <v>69</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="AO1" s="1" t="s">
         <v>20</v>
@@ -821,7 +821,7 @@
         <v>40</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>30</v>
@@ -899,7 +899,7 @@
         <v>70</v>
       </c>
       <c r="AN2" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="AO2" s="2" t="s">
         <v>39</v>

</xml_diff>